<commit_message>
Complete update to reflect changes for IATR&D
</commit_message>
<xml_diff>
--- a/content/previous-conferences/11th-international-conference/papers/icrat_papers_summary.xlsx
+++ b/content/previous-conferences/11th-international-conference/papers/icrat_papers_summary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="159">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -34,6 +34,12 @@
     <t xml:space="preserve">paper</t>
   </si>
   <si>
+    <t xml:space="preserve">presentation_ext</t>
+  </si>
+  <si>
+    <t xml:space="preserve">presentation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Track</t>
   </si>
   <si>
@@ -73,6 +79,9 @@
     <t xml:space="preserve">Decision Support System for Shift Managers based on finite state Markov chains</t>
   </si>
   <si>
+    <t xml:space="preserve">pptx</t>
+  </si>
+  <si>
     <t xml:space="preserve">Human Performance</t>
   </si>
   <si>
@@ -80,6 +89,9 @@
   </si>
   <si>
     <t xml:space="preserve">Air Traffic Management Response to Vertiport Closure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Sinan Abdulhak, Anthony Carvette, Kate Shen, Robert Goldman, Bill Tuck and Max Li</t>
@@ -683,20 +695,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D70" activeCellId="0" sqref="D70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="60"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="60.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="60.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="53.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -715,11 +728,17 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -727,23 +746,25 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A2,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_3.pdf</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>11</v>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -751,20 +772,22 @@
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A3,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_5.pdf</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>14</v>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -772,41 +795,55 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A4,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_6.pdf</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+      <c r="F4" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A4,".",E4)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_6.pptx</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D5" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A5,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_7.pdf</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>10</v>
+      <c r="E5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A5,".",E5)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_7.pdf</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -814,20 +851,27 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A6,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_9.pdf</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="F6" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A6,".",E6)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_9.pptx</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -835,20 +879,27 @@
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A7,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_10.pdf</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>25</v>
+      <c r="E7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A7,".",E7)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_10.pptx</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -856,20 +907,27 @@
         <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D8" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A8,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_11.pdf</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>28</v>
+        <v>23</v>
+      </c>
+      <c r="F8" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A8,".",E8)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_11.pdf</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -877,20 +935,22 @@
         <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D9" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A9,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_12.pdf</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>31</v>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -898,20 +958,22 @@
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D10" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A10,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_13.pdf</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>34</v>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -919,20 +981,27 @@
         <v>14</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D11" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A11,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_14.pdf</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>14</v>
+      <c r="E11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A11,".",E11)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_14.pptx</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -940,20 +1009,22 @@
         <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D12" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A12,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_15.pdf</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>17</v>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -961,41 +1032,50 @@
         <v>17</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D13" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A13,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_17.pdf</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
         <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D14" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A14,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_19.pdf</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="F14" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A14,".",E14)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_19.pdf</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1003,20 +1083,22 @@
         <v>20</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D15" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A15,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_20.pdf</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>31</v>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1024,20 +1106,27 @@
         <v>23</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D16" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A16,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_23.pdf</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>31</v>
+        <v>19</v>
+      </c>
+      <c r="F16" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A16,".",E16)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_23.pptx</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1045,20 +1134,27 @@
         <v>25</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D17" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A17,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_25.pdf</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>25</v>
+      <c r="E17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A17,".",E17)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_25.pdf</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1066,20 +1162,27 @@
         <v>26</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D18" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A18,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_26.pdf</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>10</v>
+        <v>19</v>
+      </c>
+      <c r="F18" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A18,".",E18)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_26.pptx</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1087,20 +1190,27 @@
         <v>30</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D19" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A19,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_30.pdf</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>25</v>
+      <c r="E19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A19,".",E19)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_30.pptx</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1108,20 +1218,27 @@
         <v>31</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D20" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A20,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_31.pdf</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="F20" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A20,".",E20)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_31.pptx</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1129,20 +1246,27 @@
         <v>32</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D21" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A21,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_32.pdf</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>25</v>
+      <c r="E21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A21,".",E21)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_32.pptx</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1150,20 +1274,22 @@
         <v>33</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D22" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A22,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_33.pdf</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>59</v>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1171,20 +1297,27 @@
         <v>34</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D23" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A23,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_34.pdf</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>25</v>
+      <c r="E23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A23,".",E23)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_34.pptx</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1192,20 +1325,27 @@
         <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D24" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A24,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_36.pdf</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>28</v>
+        <v>23</v>
+      </c>
+      <c r="F24" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A24,".",E24)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_36.pdf</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1213,20 +1353,22 @@
         <v>37</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D25" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A25,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_37.pdf</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>10</v>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1234,23 +1376,30 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D26" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A26,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_38.pdf</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>11</v>
+        <v>23</v>
+      </c>
+      <c r="F26" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A26,".",E26)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_38.pdf</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1258,20 +1407,22 @@
         <v>39</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D27" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A27,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_39.pdf</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>17</v>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1279,20 +1430,27 @@
         <v>40</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D28" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A28,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_40.pdf</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>10</v>
+        <v>19</v>
+      </c>
+      <c r="F28" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A28,".",E28)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_40.pptx</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1300,20 +1458,27 @@
         <v>41</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D29" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A29,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_41.pdf</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>17</v>
+      <c r="E29" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A29,".",E29)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_41.pdf</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1321,20 +1486,27 @@
         <v>42</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D30" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A30,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_42.pdf</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="0" t="s">
-        <v>59</v>
+        <v>19</v>
+      </c>
+      <c r="F30" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A30,".",E30)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_42.pptx</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1342,20 +1514,27 @@
         <v>44</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D31" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A31,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_44.pdf</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>25</v>
+      <c r="E31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A31,".",E31)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_44.pptx</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1363,20 +1542,27 @@
         <v>46</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D32" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A32,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_46.pdf</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="F32" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A32,".",E32)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_46.pptx</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1384,23 +1570,30 @@
         <v>47</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D33" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A33,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_47.pdf</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" s="0" t="s">
-        <v>11</v>
+      <c r="E33" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A33,".",E33)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_47.pptx</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1408,20 +1601,22 @@
         <v>51</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D34" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A34,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_51.pdf</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>28</v>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1429,20 +1624,27 @@
         <v>52</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D35" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A35,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_52.pdf</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>28</v>
+      <c r="E35" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A35,".",E35)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_52.pdf</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1450,20 +1652,27 @@
         <v>53</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D36" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A36,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_53.pdf</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="F36" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A36,".",E36)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_53.pptx</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1471,20 +1680,22 @@
         <v>55</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D37" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A37,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_55.pdf</v>
       </c>
-      <c r="E37" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="0" t="s">
-        <v>59</v>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1492,20 +1703,27 @@
         <v>56</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D38" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A38,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_56.pdf</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="F38" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A38,".",E38)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_56.pdf</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1513,20 +1731,27 @@
         <v>58</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D39" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A39,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_58.pdf</v>
       </c>
-      <c r="E39" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F39" s="0" t="s">
-        <v>25</v>
+      <c r="E39" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A39,".",E39)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_58.pptx</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1534,23 +1759,30 @@
         <v>61</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D40" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A40,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_61.pdf</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="G40" s="0" t="s">
-        <v>11</v>
+        <v>23</v>
+      </c>
+      <c r="F40" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A40,".",E40)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_61.pdf</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="I40" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1558,20 +1790,27 @@
         <v>62</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D41" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A41,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_62.pdf</v>
       </c>
-      <c r="E41" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="0" t="s">
-        <v>59</v>
+      <c r="E41" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A41,".",E41)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_62.pptx</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" s="0" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1579,20 +1818,27 @@
         <v>63</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D42" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A42,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_63.pdf</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F42" s="0" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="F42" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A42,".",E42)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_63.pptx</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1600,20 +1846,27 @@
         <v>64</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D43" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A43,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_64.pdf</v>
       </c>
-      <c r="E43" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="0" t="s">
-        <v>59</v>
+      <c r="E43" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F43" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A43,".",E43)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_64.pdf</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1621,41 +1874,55 @@
         <v>65</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D44" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A44,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_65.pdf</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F44" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+      <c r="F44" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A44,".",E44)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_65.pptx</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H44" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="n">
         <v>66</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D45" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A45,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_66.pdf</v>
       </c>
-      <c r="E45" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>25</v>
+      <c r="E45" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F45" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A45,".",E45)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_66.pdf</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H45" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1663,20 +1930,22 @@
         <v>67</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D46" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A46,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_67.pdf</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F46" s="0" t="s">
-        <v>14</v>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1684,20 +1953,22 @@
         <v>68</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D47" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A47,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_68.pdf</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F47" s="0" t="s">
-        <v>25</v>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H47" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1705,20 +1976,27 @@
         <v>69</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D48" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A48,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_69.pdf</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F48" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="F48" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A48,".",E48)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_69.pptx</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H48" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1726,20 +2004,27 @@
         <v>70</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D49" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A49,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_70.pdf</v>
       </c>
-      <c r="E49" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F49" s="0" t="s">
-        <v>31</v>
+      <c r="E49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F49" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A49,".",E49)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_70.pdf</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H49" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1747,20 +2032,22 @@
         <v>71</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D50" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A50,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_71.pdf</v>
       </c>
-      <c r="E50" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F50" s="0" t="s">
-        <v>25</v>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H50" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1768,23 +2055,30 @@
         <v>72</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D51" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A51,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_72.pdf</v>
       </c>
-      <c r="E51" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F51" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="G51" s="0" t="s">
-        <v>11</v>
+      <c r="E51" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F51" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A51,".",E51)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_72.pdf</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H51" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="I51" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1792,20 +2086,22 @@
         <v>73</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D52" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A52,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_73.pdf</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F52" s="0" t="s">
-        <v>25</v>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H52" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1813,20 +2109,22 @@
         <v>74</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D53" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A53,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_74.pdf</v>
       </c>
-      <c r="E53" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F53" s="0" t="s">
-        <v>59</v>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H53" s="0" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1834,20 +2132,22 @@
         <v>75</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D54" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A54,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_75.pdf</v>
       </c>
-      <c r="E54" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F54" s="0" t="s">
-        <v>34</v>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H54" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1855,20 +2155,27 @@
         <v>76</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D55" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A55,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_76.pdf</v>
       </c>
-      <c r="E55" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F55" s="0" t="s">
-        <v>10</v>
+      <c r="E55" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F55" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A55,".",E55)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_76.pdf</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H55" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1876,20 +2183,27 @@
         <v>78</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D56" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A56,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_78.pdf</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="F56" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A56,".",E56)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_78.pdf</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H56" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1897,20 +2211,27 @@
         <v>79</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D57" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A57,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_79.pdf</v>
       </c>
-      <c r="E57" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F57" s="0" t="s">
-        <v>31</v>
+      <c r="E57" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F57" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A57,".",E57)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_79.pdf</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H57" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1918,20 +2239,27 @@
         <v>80</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D58" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A58,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_80.pdf</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F58" s="0" t="s">
-        <v>34</v>
+        <v>23</v>
+      </c>
+      <c r="F58" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A58,".",E58)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_80.pdf</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H58" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1939,20 +2267,27 @@
         <v>82</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D59" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A59,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_82.pdf</v>
       </c>
-      <c r="E59" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F59" s="0" t="s">
-        <v>25</v>
+      <c r="E59" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F59" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A59,".",E59)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_82.pptx</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H59" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1960,20 +2295,27 @@
         <v>83</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D60" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A60,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_83.pdf</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F60" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="F60" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A60,".",E60)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_83.pptx</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H60" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1981,20 +2323,22 @@
         <v>84</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D61" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A61,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_84.pdf</v>
       </c>
-      <c r="E61" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F61" s="0" t="s">
-        <v>34</v>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H61" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2002,20 +2346,24 @@
         <v>87</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D62" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A62,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_87.pdf</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F62" s="0" t="s">
-        <v>31</v>
+        <v>23</v>
+      </c>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H62" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2023,20 +2371,22 @@
         <v>88</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D63" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A63,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_88.pdf</v>
       </c>
-      <c r="E63" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F63" s="0" t="s">
-        <v>17</v>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H63" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2044,23 +2394,30 @@
         <v>91</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D64" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A64,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_91.pdf</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F64" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="G64" s="0" t="s">
-        <v>11</v>
+        <v>23</v>
+      </c>
+      <c r="F64" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A64,".",E64)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_91.pdf</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H64" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I64" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2068,20 +2425,27 @@
         <v>92</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D65" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A65,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_92.pdf</v>
       </c>
-      <c r="E65" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F65" s="0" t="s">
-        <v>10</v>
+      <c r="E65" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F65" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A65,".",E65)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_92.pdf</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H65" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2089,20 +2453,22 @@
         <v>93</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D66" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A66,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_93.pdf</v>
       </c>
-      <c r="E66" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F66" s="0" t="s">
-        <v>28</v>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H66" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2110,20 +2476,22 @@
         <v>94</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D67" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A67,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_94.pdf</v>
       </c>
-      <c r="E67" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F67" s="0" t="s">
-        <v>25</v>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H67" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2131,20 +2499,22 @@
         <v>95</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D68" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A68,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_95.pdf</v>
       </c>
-      <c r="E68" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F68" s="0" t="s">
-        <v>34</v>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H68" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2152,20 +2522,22 @@
         <v>97</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D69" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A69,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_97.pdf</v>
       </c>
-      <c r="E69" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F69" s="0" t="s">
-        <v>14</v>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H69" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2173,23 +2545,30 @@
         <v>99</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D70" s="2" t="str">
         <f aca="false">_xlfn.CONCAT("/seminarContent/2024/papers/ICRAT2024_paper_",A70,".pdf")</f>
         <v>/seminarContent/2024/papers/ICRAT2024_paper_99.pdf</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F70" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G70" s="0" t="s">
-        <v>11</v>
+        <v>23</v>
+      </c>
+      <c r="F70" s="2" t="str">
+        <f aca="false">_xlfn.CONCAT("/seminarContent/2024/presentations/ICRAT2024_Presentation_",A70,".",E70)</f>
+        <v>/seminarContent/2024/presentations/ICRAT2024_Presentation_99.pdf</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I70" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>